<commit_message>
delete excess and wrong stations in tram1
</commit_message>
<xml_diff>
--- a/data/am_tram1_name.xlsx
+++ b/data/am_tram1_name.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\UTNCE\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABEB83CB-0107-4A40-B9E7-FAF430ED6D75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7F0667A-EF39-4E90-AB52-4392E56244BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="952" yWindow="1477" windowWidth="16200" windowHeight="9308" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Dapperstraat</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Beukenweg</t>
   </si>
   <si>
-    <t>Korte`s Gravesandestraat</t>
-  </si>
-  <si>
     <t>Weesperplein</t>
   </si>
   <si>
@@ -54,73 +51,77 @@
     <t>Leidseplein</t>
   </si>
   <si>
-    <t>Stadhouderskade</t>
+    <t>Rhijnvis Feithstraat</t>
+  </si>
+  <si>
+    <t>Surinameplein</t>
+  </si>
+  <si>
+    <t>Derkinderenstraat</t>
+  </si>
+  <si>
+    <t>Station Lelylaan</t>
+  </si>
+  <si>
+    <t>Johan Huizingalaan</t>
+  </si>
+  <si>
+    <t>Meer en Vaart</t>
+  </si>
+  <si>
+    <t>Louis Davidsstraat</t>
+  </si>
+  <si>
+    <t>Hoekenes</t>
+  </si>
+  <si>
+    <t>Baden Powellweg</t>
+  </si>
+  <si>
+    <t>Ecuplein</t>
+  </si>
+  <si>
+    <t>Inaristraat</t>
+  </si>
+  <si>
+    <t>Pilatus</t>
+  </si>
+  <si>
+    <t>Matterhorn</t>
+  </si>
+  <si>
+    <t>Muiderpoortstation</t>
   </si>
   <si>
     <t>Eerste Constantijn Huygensstraat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Korte 's-Gravesandestraat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Jan Pieter Heijestraat</t>
-  </si>
-  <si>
-    <t>Rhijnvis Feithstraat</t>
-  </si>
-  <si>
-    <t>Overtoomsesluis</t>
-  </si>
-  <si>
-    <t>Surinameplein</t>
-  </si>
-  <si>
-    <t>Derkinderenstraat</t>
-  </si>
-  <si>
-    <t>Station Lelylaan</t>
-  </si>
-  <si>
-    <t>Johan Huizingalaan</t>
-  </si>
-  <si>
-    <t>Piet Wiedijkstraat</t>
-  </si>
-  <si>
-    <t>Meer en Vaart</t>
-  </si>
-  <si>
-    <t>Louis Davidsstraat</t>
-  </si>
-  <si>
-    <t>Hoekenes</t>
-  </si>
-  <si>
-    <t>Baden Powellweg</t>
-  </si>
-  <si>
-    <t>Ecuplein</t>
-  </si>
-  <si>
-    <t>Inaristraat</t>
-  </si>
-  <si>
-    <t>Pilatus</t>
-  </si>
-  <si>
-    <t>Matterhorn</t>
-  </si>
-  <si>
-    <t>Muiderpoortstation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -148,7 +149,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -426,155 +427,141 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A28"/>
+  <dimension ref="A1:A25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A16" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A19" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A20" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A21" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A22" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A23" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A24" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A25" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>26</v>
-      </c>
-    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
get tram1, id_pairs and shortest path is wrong
</commit_message>
<xml_diff>
--- a/data/am_tram1_name.xlsx
+++ b/data/am_tram1_name.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\UTNCE\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7F0667A-EF39-4E90-AB52-4392E56244BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D136196-EC46-427D-9E15-59FFFB933C5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="952" yWindow="1477" windowWidth="16200" windowHeight="9308" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5258" yWindow="2107" windowWidth="16200" windowHeight="9308" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,9 +45,6 @@
     <t>Weteringcircuit</t>
   </si>
   <si>
-    <t>Spiegelgracht</t>
-  </si>
-  <si>
     <t>Leidseplein</t>
   </si>
   <si>
@@ -103,6 +100,9 @@
   <si>
     <t>Jan Pieter Heijestraat</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rijksmuseum</t>
   </si>
 </sst>
 </file>
@@ -429,15 +429,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="29.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.4">
@@ -457,7 +458,7 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.4">
@@ -477,87 +478,87 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
revise am_tram1_name and related codes
</commit_message>
<xml_diff>
--- a/data/am_tram1_name.xlsx
+++ b/data/am_tram1_name.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\UTNCE\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D136196-EC46-427D-9E15-59FFFB933C5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD2B9FC5-4535-4E1B-991A-425E1B94D50B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5258" yWindow="2107" windowWidth="16200" windowHeight="9308" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4215" yWindow="3090" windowWidth="21600" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,9 +42,6 @@
     <t>Frederiksplein</t>
   </si>
   <si>
-    <t>Weteringcircuit</t>
-  </si>
-  <si>
     <t>Leidseplein</t>
   </si>
   <si>
@@ -103,23 +100,26 @@
   </si>
   <si>
     <t>Rijksmuseum</t>
+  </si>
+  <si>
+    <t>Vijzelgracht</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -149,7 +149,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -429,136 +429,138 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:1">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
       <c r="A6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:1">
       <c r="A7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:1">
       <c r="A8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A10" t="s">
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A13" t="s">
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A14" t="s">
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A15" t="s">
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A16" t="s">
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A17" t="s">
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A18" t="s">
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A19" t="s">
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A20" t="s">
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A21" t="s">
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A22" t="s">
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A23" t="s">
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A24" t="s">
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A25" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>